<commit_message>
Notes on 17-02_26 meeting
</commit_message>
<xml_diff>
--- a/literature-management.xlsx
+++ b/literature-management.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jay/phd/papers/sok - a survey on software power monitoring tools/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E04D725B-A84F-DC47-B77A-8EBB90C1CC93}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9EB4E29-021A-B949-988C-5760C58B83E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="160" yWindow="920" windowWidth="29920" windowHeight="18560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="160" yWindow="920" windowWidth="29920" windowHeight="18560" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tools" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="116">
   <si>
     <t>Year</t>
   </si>
@@ -399,6 +399,9 @@
   </si>
   <si>
     <t>open-source</t>
+  </si>
+  <si>
+    <t>case studies</t>
   </si>
 </sst>
 </file>
@@ -1169,8 +1172,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:K44"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3:C7"/>
+    <sheetView topLeftCell="B2" workbookViewId="0">
+      <selection activeCell="C35" sqref="C35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1670,7 +1673,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B2:J21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="B3" sqref="B3:B7"/>
     </sheetView>
   </sheetViews>
@@ -1976,10 +1979,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="B2:AN31"/>
+  <dimension ref="B2:AO31"/>
   <sheetViews>
-    <sheetView zoomScale="89" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" topLeftCell="L1" zoomScale="89" workbookViewId="0">
+      <selection activeCell="N5" sqref="N5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2026,7 +2029,7 @@
     <col min="42" max="42" width="29" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:40" ht="24" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:41" ht="24" x14ac:dyDescent="0.3">
       <c r="B2" s="37" t="s">
         <v>20</v>
       </c>
@@ -2079,7 +2082,7 @@
       <c r="AM2" s="7"/>
       <c r="AN2" s="8"/>
     </row>
-    <row r="3" spans="2:40" ht="54" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:41" ht="54" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B3" s="37"/>
       <c r="C3" s="60" t="s">
         <v>26</v>
@@ -2165,8 +2168,11 @@
       <c r="AN3" s="55" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="4" spans="2:40" ht="81" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="AO3" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="4" spans="2:41" ht="81" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="40"/>
       <c r="C4" s="58" t="s">
         <v>59</v>
@@ -2247,7 +2253,7 @@
       <c r="AM4" s="50"/>
       <c r="AN4" s="50"/>
     </row>
-    <row r="5" spans="2:40" ht="17" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:41" ht="17" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="B5" s="73" t="s">
         <v>27</v>
       </c>
@@ -2326,7 +2332,7 @@
       <c r="AM5" s="39"/>
       <c r="AN5" s="4"/>
     </row>
-    <row r="6" spans="2:40" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:41" x14ac:dyDescent="0.2">
       <c r="B6" s="74" t="s">
         <v>31</v>
       </c>
@@ -2369,7 +2375,7 @@
       <c r="AM6" s="4"/>
       <c r="AN6" s="4"/>
     </row>
-    <row r="7" spans="2:40" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:41" x14ac:dyDescent="0.2">
       <c r="B7" s="74" t="s">
         <v>51</v>
       </c>
@@ -2419,7 +2425,7 @@
       <c r="AM7" s="4"/>
       <c r="AN7" s="4"/>
     </row>
-    <row r="8" spans="2:40" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:41" x14ac:dyDescent="0.2">
       <c r="B8" s="74" t="s">
         <v>39</v>
       </c>
@@ -2462,7 +2468,7 @@
       <c r="AM8" s="4"/>
       <c r="AN8" s="4"/>
     </row>
-    <row r="9" spans="2:40" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:41" x14ac:dyDescent="0.2">
       <c r="B9" s="75" t="s">
         <v>32</v>
       </c>
@@ -2505,7 +2511,7 @@
       <c r="AM9" s="4"/>
       <c r="AN9" s="4"/>
     </row>
-    <row r="10" spans="2:40" x14ac:dyDescent="0.2">
+    <row r="10" spans="2:41" x14ac:dyDescent="0.2">
       <c r="B10" s="4"/>
       <c r="C10" s="4"/>
       <c r="D10" s="4"/>
@@ -2546,7 +2552,7 @@
       <c r="AM10" s="4"/>
       <c r="AN10" s="4"/>
     </row>
-    <row r="11" spans="2:40" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:41" x14ac:dyDescent="0.2">
       <c r="B11" s="4"/>
       <c r="C11" s="4"/>
       <c r="D11" s="4"/>
@@ -2587,7 +2593,7 @@
       <c r="AM11" s="4"/>
       <c r="AN11" s="4"/>
     </row>
-    <row r="12" spans="2:40" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:41" x14ac:dyDescent="0.2">
       <c r="B12" s="4"/>
       <c r="C12" s="4"/>
       <c r="D12" s="4"/>
@@ -2628,7 +2634,7 @@
       <c r="AM12" s="4"/>
       <c r="AN12" s="4"/>
     </row>
-    <row r="13" spans="2:40" x14ac:dyDescent="0.2">
+    <row r="13" spans="2:41" x14ac:dyDescent="0.2">
       <c r="B13" s="4"/>
       <c r="C13" s="4"/>
       <c r="D13" s="4"/>
@@ -2669,7 +2675,7 @@
       <c r="AM13" s="4"/>
       <c r="AN13" s="4"/>
     </row>
-    <row r="14" spans="2:40" x14ac:dyDescent="0.2">
+    <row r="14" spans="2:41" x14ac:dyDescent="0.2">
       <c r="B14" s="4"/>
       <c r="C14" s="4"/>
       <c r="D14" s="4"/>
@@ -2710,7 +2716,7 @@
       <c r="AM14" s="4"/>
       <c r="AN14" s="4"/>
     </row>
-    <row r="15" spans="2:40" x14ac:dyDescent="0.2">
+    <row r="15" spans="2:41" x14ac:dyDescent="0.2">
       <c r="B15" s="4"/>
       <c r="C15" s="4"/>
       <c r="D15" s="4"/>
@@ -2751,7 +2757,7 @@
       <c r="AM15" s="4"/>
       <c r="AN15" s="4"/>
     </row>
-    <row r="16" spans="2:40" x14ac:dyDescent="0.2">
+    <row r="16" spans="2:41" x14ac:dyDescent="0.2">
       <c r="B16" s="4"/>
       <c r="C16" s="4"/>
       <c r="D16" s="4"/>

</xml_diff>